<commit_message>
:up: Fix privacy and read-only settings
</commit_message>
<xml_diff>
--- a/tests/testthat/excel/gyokaikyo_dummy_maaji.xlsx
+++ b/tests/testthat/excel/gyokaikyo_dummy_maaji.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akihiro\Documents\zaitaku\202003\dummydata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akihiro\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66835175-0AD6-4D82-8109-0B06FD5A2ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{443896EA-CDFD-440E-8870-3DE6F08EB210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{830C94F2-9979-486B-8456-AF580F2FA102}"/>
+    <workbookView xWindow="17775" yWindow="1710" windowWidth="21600" windowHeight="11325" xr2:uid="{830C94F2-9979-486B-8456-AF580F2FA102}"/>
   </bookViews>
   <sheets>
     <sheet name="鹿児島" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
:up: Remove privacy data again
</commit_message>
<xml_diff>
--- a/tests/testthat/excel/gyokaikyo_dummy_maaji.xlsx
+++ b/tests/testthat/excel/gyokaikyo_dummy_maaji.xlsx
@@ -3,15 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <fileSharing readOnlyRecommended="1"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akihiro\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{443896EA-CDFD-440E-8870-3DE6F08EB210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB703744-0618-4B84-8EE2-2675F01871A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17775" yWindow="1710" windowWidth="21600" windowHeight="11325" xr2:uid="{830C94F2-9979-486B-8456-AF580F2FA102}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{830C94F2-9979-486B-8456-AF580F2FA102}"/>
   </bookViews>
   <sheets>
     <sheet name="鹿児島" sheetId="2" r:id="rId1"/>

</xml_diff>